<commit_message>
Docs in Final upload are relevant for final model
</commit_message>
<xml_diff>
--- a/df_scores.xlsx
+++ b/df_scores.xlsx
@@ -469,27 +469,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0.67 0.84 0.67 0.71 0.86 0.73 0.69 0.69 0.8  0.7 ]</t>
+          <t>[0.69 0.86 0.71 0.69 0.76 0.71 0.69 0.73 0.78 0.72]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[0.69 0.85 0.65 0.58 0.76 0.6  0.56 0.6  0.8  0.76]</t>
+          <t>[0.77 0.85 0.73 0.65 0.64 0.6  0.6  0.76 0.76 0.8 ]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[0.64 0.84 0.68 0.84 0.96 0.85 0.81 0.77 0.8  0.64]</t>
+          <t>[0.6  0.88 0.68 0.72 0.88 0.81 0.77 0.69 0.8  0.64]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[0.75 0.89 0.77 0.74 0.93 0.77 0.79 0.74 0.9  0.82]</t>
+          <t>[0.79 0.91 0.82 0.75 0.94 0.76 0.76 0.76 0.86 0.83]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[0.51 0.78 0.54 0.48 0.86 0.53 0.58 0.48 0.79 0.64]</t>
+          <t>[0.57 0.81 0.65 0.5  0.87 0.53 0.52 0.52 0.73 0.65]</t>
         </is>
       </c>
     </row>
@@ -501,27 +501,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0.69 0.78 0.69 0.76 0.84 0.63 0.69 0.69 0.82 0.78]</t>
+          <t>[0.73 0.75 0.65 0.75 0.88 0.63 0.67 0.69 0.82 0.74]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[0.73 0.77 0.65 0.69 0.76 0.52 0.6  0.48 0.8  0.76]</t>
+          <t>[0.65 0.69 0.54 0.73 0.8  0.56 0.6  0.52 0.8  0.72]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[0.64 0.8  0.72 0.84 0.92 0.73 0.77 0.88 0.84 0.8 ]</t>
+          <t>[0.8  0.8  0.76 0.76 0.96 0.69 0.73 0.85 0.84 0.76]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[0.77 0.84 0.74 0.84 0.95 0.69 0.77 0.77 0.88 0.84]</t>
+          <t>[0.82 0.79 0.72 0.8  0.95 0.7  0.76 0.76 0.87 0.84]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.54 0.68 0.48 0.68 0.9  0.38 0.54 0.54 0.75 0.69]</t>
+          <t>[0.63 0.58 0.43 0.61 0.9  0.4  0.52 0.52 0.75 0.68]</t>
         </is>
       </c>
     </row>
@@ -579,27 +579,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.73 +/- 0.07</t>
+          <t>0.73 +/- 0.05</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.68 +/- 0.1</t>
+          <t>0.72 +/- 0.08</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.78 +/- 0.1</t>
+          <t>0.75 +/- 0.09</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.81 +/- 0.07</t>
+          <t>0.82 +/- 0.06</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.62 +/- 0.14</t>
+          <t>0.64 +/- 0.13</t>
         </is>
       </c>
     </row>
@@ -611,27 +611,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.74 +/- 0.07</t>
+          <t>0.73 +/- 0.07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.68 +/- 0.11</t>
+          <t>0.66 +/- 0.1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.79 +/- 0.08</t>
+          <t>0.8 +/- 0.07</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.81 +/- 0.07</t>
+          <t>0.8 +/- 0.07</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.62 +/- 0.14</t>
+          <t>0.6 +/- 0.14</t>
         </is>
       </c>
     </row>

</xml_diff>